<commit_message>
update html, dashboard, add ellipse
</commit_message>
<xml_diff>
--- a/data/tf1.xlsx
+++ b/data/tf1.xlsx
@@ -525,7 +525,7 @@
   <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -591,7 +591,7 @@
         <v>2</v>
       </c>
       <c r="J2" s="19">
-        <v>1000</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:10">

</xml_diff>